<commit_message>
Ikke lavet det store
</commit_message>
<xml_diff>
--- a/TIMES-AZ/SysSettings.xlsx
+++ b/TIMES-AZ/SysSettings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TIMES models\TIMES_AZ\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c0ee8d5d29f1698f/Desktop/GitHub/Bachelor_Git/TIMES-AZ/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D251032D-EB69-47F3-A6B4-B355B57B27ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19884" yWindow="684" windowWidth="21012" windowHeight="14256" tabRatio="853" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="853" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Region-Time Slices" sheetId="16" r:id="rId1"/>
@@ -4023,10 +4023,10 @@
     <xf numFmtId="2" fontId="0" fillId="9" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="11" borderId="11" xfId="11" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="21">
     <cellStyle name="5x indented GHG Textfiels" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -4034,8 +4034,8 @@
     <cellStyle name="AggOrange9_CRFReport-template" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="CustomizationCells" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
     <cellStyle name="Euro" xfId="5" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
-    <cellStyle name="Hyperlink" xfId="20" builtinId="8"/>
     <cellStyle name="InputCells" xfId="6" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Link" xfId="20" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 10" xfId="7" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
     <cellStyle name="Normal 10 2" xfId="8" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
@@ -4046,9 +4046,9 @@
     <cellStyle name="Normal GHG Textfiels Bold" xfId="13" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
     <cellStyle name="Normal GHG-Shade" xfId="14" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
     <cellStyle name="Normale_B2020" xfId="15" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
-    <cellStyle name="Percent" xfId="16" builtinId="5"/>
+    <cellStyle name="Procent" xfId="16" builtinId="5"/>
+    <cellStyle name="Standard_Sce_D_Extraction" xfId="17" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
     <cellStyle name="Standaard_Blad1" xfId="19" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
-    <cellStyle name="Standard_Sce_D_Extraction" xfId="17" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
     <cellStyle name="Обычный_CRF2002 (1)" xfId="18" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -4114,7 +4114,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -4439,21 +4439,21 @@
   </sheetPr>
   <dimension ref="A3:R39"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.109375" customWidth="1"/>
-    <col min="2" max="2" width="19.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="2.109375" customWidth="1"/>
-    <col min="5" max="5" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.08984375" customWidth="1"/>
+    <col min="2" max="2" width="19.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="2.08984375" customWidth="1"/>
+    <col min="5" max="5" width="12.08984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.54296875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" ht="13" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
       <c r="B3" s="7" t="s">
         <v>6</v>
@@ -4464,7 +4464,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:18" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" ht="13" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="8" t="s">
         <v>12</v>
@@ -4657,7 +4657,7 @@
       <c r="O12" s="12"/>
       <c r="P12" s="12"/>
     </row>
-    <row r="13" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" ht="13" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -4665,7 +4665,7 @@
       <c r="O13" s="13"/>
       <c r="P13" s="14"/>
     </row>
-    <row r="14" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" ht="13" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -4673,7 +4673,7 @@
       <c r="O14" s="13"/>
       <c r="P14" s="14"/>
     </row>
-    <row r="15" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" ht="13" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
       <c r="B15" s="114"/>
       <c r="C15" s="3"/>
@@ -4681,28 +4681,28 @@
       <c r="O15" s="13"/>
       <c r="P15" s="14"/>
     </row>
-    <row r="16" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" ht="13" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="B16" s="115"/>
       <c r="C16" s="115"/>
       <c r="O16" s="13"/>
       <c r="P16" s="14"/>
     </row>
-    <row r="17" spans="1:16" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" ht="13" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
       <c r="B17" s="115"/>
       <c r="C17" s="115"/>
       <c r="O17" s="12"/>
       <c r="P17" s="12"/>
     </row>
-    <row r="18" spans="1:16" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" ht="13" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
       <c r="B18" s="115"/>
       <c r="C18" s="115"/>
       <c r="O18" s="12"/>
       <c r="P18" s="12"/>
     </row>
-    <row r="19" spans="1:16" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" ht="13" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
       <c r="B19" s="115"/>
       <c r="C19" s="115"/>
@@ -4781,29 +4781,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B3:K57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:11" ht="13" x14ac:dyDescent="0.3">
       <c r="B3" s="17" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>2010</v>
       </c>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:11" ht="13" x14ac:dyDescent="0.3">
       <c r="B7" s="17" t="s">
         <v>32</v>
       </c>
@@ -4814,7 +4814,7 @@
       <c r="I7" s="69"/>
       <c r="J7" s="69"/>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>44</v>
       </c>
@@ -4823,23 +4823,23 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:11" ht="13" x14ac:dyDescent="0.3">
       <c r="B10" s="71" t="str">
         <f ca="1">IF(VEDA2,"~DefaultYear",T(0))</f>
         <v>~DefaultYear</v>
       </c>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B11" s="70">
         <v>2010</v>
       </c>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:11" ht="13" x14ac:dyDescent="0.3">
       <c r="B15" s="17" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B16" s="64" t="s">
         <v>44</v>
       </c>
@@ -4849,17 +4849,17 @@
       <c r="D16" s="65" t="s">
         <v>1014</v>
       </c>
-      <c r="I16" s="151" t="s">
+      <c r="I16" s="149" t="s">
         <v>44</v>
       </c>
-      <c r="J16" s="151" t="s">
+      <c r="J16" s="149" t="s">
         <v>1013</v>
       </c>
       <c r="K16" s="89" t="s">
         <v>1014</v>
       </c>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B17" s="9">
         <v>1</v>
       </c>
@@ -4879,7 +4879,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B18" s="9">
         <v>3</v>
       </c>
@@ -4899,7 +4899,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B19" s="9">
         <v>4</v>
       </c>
@@ -4919,7 +4919,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B20" s="9">
         <v>5</v>
       </c>
@@ -4939,7 +4939,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B21" s="9">
         <v>5</v>
       </c>
@@ -4959,7 +4959,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B22" s="9">
         <v>5</v>
       </c>
@@ -4979,7 +4979,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B23" s="9">
         <v>5</v>
       </c>
@@ -4999,7 +4999,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B24" s="9">
         <v>5</v>
       </c>
@@ -5019,7 +5019,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B25" s="9">
         <v>5</v>
       </c>
@@ -5039,7 +5039,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:11" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B26" s="9">
         <v>5</v>
       </c>
@@ -5308,7 +5308,7 @@
       <c r="C44" s="9">
         <v>1</v>
       </c>
-      <c r="D44" s="152"/>
+      <c r="D44" s="150"/>
       <c r="J44">
         <v>2037</v>
       </c>
@@ -5317,7 +5317,7 @@
       <c r="C45" s="9">
         <v>1</v>
       </c>
-      <c r="D45" s="152"/>
+      <c r="D45" s="150"/>
       <c r="J45">
         <v>2038</v>
       </c>
@@ -5326,7 +5326,7 @@
       <c r="C46" s="9">
         <v>1</v>
       </c>
-      <c r="D46" s="152"/>
+      <c r="D46" s="150"/>
       <c r="J46">
         <v>2039</v>
       </c>
@@ -5335,7 +5335,7 @@
       <c r="C47" s="9">
         <v>1</v>
       </c>
-      <c r="D47" s="152"/>
+      <c r="D47" s="150"/>
       <c r="J47">
         <v>2040</v>
       </c>
@@ -5344,7 +5344,7 @@
       <c r="C48" s="9">
         <v>1</v>
       </c>
-      <c r="D48" s="152"/>
+      <c r="D48" s="150"/>
       <c r="J48">
         <v>2041</v>
       </c>
@@ -5353,7 +5353,7 @@
       <c r="C49" s="9">
         <v>1</v>
       </c>
-      <c r="D49" s="152"/>
+      <c r="D49" s="150"/>
       <c r="J49">
         <v>2042</v>
       </c>
@@ -5362,7 +5362,7 @@
       <c r="C50" s="9">
         <v>1</v>
       </c>
-      <c r="D50" s="152"/>
+      <c r="D50" s="150"/>
       <c r="J50">
         <v>2043</v>
       </c>
@@ -5371,7 +5371,7 @@
       <c r="C51" s="9">
         <v>1</v>
       </c>
-      <c r="D51" s="152"/>
+      <c r="D51" s="150"/>
       <c r="J51">
         <v>2044</v>
       </c>
@@ -5380,7 +5380,7 @@
       <c r="C52" s="9">
         <v>1</v>
       </c>
-      <c r="D52" s="152"/>
+      <c r="D52" s="150"/>
       <c r="J52">
         <v>2045</v>
       </c>
@@ -5389,7 +5389,7 @@
       <c r="C53" s="9">
         <v>1</v>
       </c>
-      <c r="D53" s="152"/>
+      <c r="D53" s="150"/>
       <c r="J53">
         <v>2046</v>
       </c>
@@ -5398,7 +5398,7 @@
       <c r="C54" s="9">
         <v>1</v>
       </c>
-      <c r="D54" s="152"/>
+      <c r="D54" s="150"/>
       <c r="J54">
         <v>2047</v>
       </c>
@@ -5407,7 +5407,7 @@
       <c r="C55" s="9">
         <v>1</v>
       </c>
-      <c r="D55" s="152"/>
+      <c r="D55" s="150"/>
       <c r="J55">
         <v>2048</v>
       </c>
@@ -5416,7 +5416,7 @@
       <c r="C56" s="9">
         <v>1</v>
       </c>
-      <c r="D56" s="152"/>
+      <c r="D56" s="150"/>
       <c r="J56">
         <v>2049</v>
       </c>
@@ -5425,7 +5425,7 @@
       <c r="C57" s="9">
         <v>1</v>
       </c>
-      <c r="D57" s="152"/>
+      <c r="D57" s="150"/>
       <c r="J57">
         <v>2050</v>
       </c>
@@ -5447,34 +5447,34 @@
       <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.88671875" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" customWidth="1"/>
-    <col min="3" max="3" width="12.44140625" customWidth="1"/>
-    <col min="4" max="4" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" customWidth="1"/>
+    <col min="1" max="1" width="2.90625" customWidth="1"/>
+    <col min="2" max="2" width="13.36328125" customWidth="1"/>
+    <col min="3" max="3" width="12.453125" customWidth="1"/>
+    <col min="4" max="4" width="13.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.36328125" customWidth="1"/>
     <col min="6" max="13" width="8" customWidth="1"/>
-    <col min="17" max="17" width="21.44140625" customWidth="1"/>
-    <col min="18" max="18" width="15.5546875" customWidth="1"/>
-    <col min="20" max="20" width="7.5546875" customWidth="1"/>
-    <col min="21" max="21" width="8.109375" customWidth="1"/>
+    <col min="17" max="17" width="21.453125" customWidth="1"/>
+    <col min="18" max="18" width="15.54296875" customWidth="1"/>
+    <col min="20" max="20" width="7.54296875" customWidth="1"/>
+    <col min="21" max="21" width="8.08984375" customWidth="1"/>
     <col min="22" max="22" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
     </row>
-    <row r="4" spans="2:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
     </row>
-    <row r="5" spans="2:24" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:24" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="17" t="str">
         <f ca="1">IF(VEDA2,"~TFM_MIG","~TFM_UPD")</f>
         <v>~TFM_MIG</v>
@@ -5596,30 +5596,30 @@
       <c r="W8" s="67"/>
       <c r="X8" s="67"/>
     </row>
-    <row r="11" spans="2:24" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:24" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B11" s="4" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="12" spans="2:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="2:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" s="5" t="s">
         <v>33</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
     </row>
-    <row r="14" spans="2:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
     </row>
-    <row r="15" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:24" ht="13" x14ac:dyDescent="0.3">
       <c r="B15" s="17" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:24" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:24" ht="13" x14ac:dyDescent="0.25">
       <c r="B16" s="8" t="s">
         <v>18</v>
       </c>
@@ -5662,19 +5662,19 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="2:13" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B21" s="4" t="s">
         <v>950</v>
       </c>
     </row>
-    <row r="23" spans="2:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:13" ht="17.5" x14ac:dyDescent="0.35">
       <c r="B23" s="5" t="s">
         <v>951</v>
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
     </row>
-    <row r="24" spans="2:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:13" ht="17.5" x14ac:dyDescent="0.35">
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
@@ -5682,12 +5682,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:13" ht="13" x14ac:dyDescent="0.3">
       <c r="B25" s="17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="2:13" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:13" ht="26" x14ac:dyDescent="0.25">
       <c r="B26" s="8" t="s">
         <v>17</v>
       </c>
@@ -5750,16 +5750,16 @@
       <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.44140625" customWidth="1"/>
-    <col min="2" max="2" width="52.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.453125" customWidth="1"/>
+    <col min="2" max="2" width="52.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:10" ht="13" x14ac:dyDescent="0.3">
       <c r="B1" s="17" t="str">
         <f ca="1">"~Scenario:"&amp;REPLACE(REPLACE($F$1,FIND(".",$F$1),100,""),1,FIND("[",$F$1),"")</f>
-        <v>~Scenario:SysSettings</v>
+        <v>~Scenario:</v>
       </c>
       <c r="C1" s="34" t="b">
         <f ca="1">NOT(ISERR(FIND(".xlsx",$F$1)))</f>
@@ -5770,17 +5770,17 @@
       </c>
       <c r="F1" s="17" t="str">
         <f ca="1">CELL("filename",$E$1)</f>
-        <v>C:\TIMES models\TIMES_AZ\[SysSettings.xlsx]Import Settings</v>
+        <v>https://d.docs.live.net/c0ee8d5d29f1698f/Desktop/GitHub/Bachelor_Git/TIMES-AZ/[SysSettings.xlsx]Import Settings</v>
       </c>
       <c r="I1" s="66"/>
       <c r="J1" s="17"/>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:10" ht="13" x14ac:dyDescent="0.3">
       <c r="B3" s="17" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="2:10" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:10" ht="13" x14ac:dyDescent="0.25">
       <c r="B4" s="18" t="s">
         <v>25</v>
       </c>
@@ -5847,30 +5847,30 @@
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.44140625" style="56" customWidth="1"/>
-    <col min="2" max="2" width="13.6640625" style="56" customWidth="1"/>
-    <col min="3" max="3" width="12.33203125" style="56" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.5546875" style="56" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.88671875" style="56" customWidth="1"/>
-    <col min="6" max="8" width="8.33203125" style="56" customWidth="1"/>
-    <col min="9" max="13" width="9.109375" style="56"/>
-    <col min="14" max="14" width="18.6640625" style="56" customWidth="1"/>
-    <col min="15" max="16384" width="9.109375" style="56"/>
+    <col min="1" max="1" width="3.453125" style="56" customWidth="1"/>
+    <col min="2" max="2" width="13.6328125" style="56" customWidth="1"/>
+    <col min="3" max="3" width="12.36328125" style="56" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.54296875" style="56" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.90625" style="56" customWidth="1"/>
+    <col min="6" max="8" width="8.36328125" style="56" customWidth="1"/>
+    <col min="9" max="13" width="9.08984375" style="56"/>
+    <col min="14" max="14" width="18.6328125" style="56" customWidth="1"/>
+    <col min="15" max="16384" width="9.08984375" style="56"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:55" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:55" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B3" s="4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="2:55" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:55" ht="13" x14ac:dyDescent="0.3">
       <c r="B5" s="94" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="2:55" ht="27.6" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:55" ht="26" x14ac:dyDescent="0.45">
       <c r="B6" s="8" t="s">
         <v>16</v>
       </c>
@@ -5944,7 +5944,7 @@
       <c r="BB6"/>
       <c r="BC6"/>
     </row>
-    <row r="7" spans="2:55" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:55" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B7" s="99"/>
       <c r="C7" s="99" t="s">
         <v>49</v>
@@ -6006,7 +6006,7 @@
       <c r="BB7"/>
       <c r="BC7"/>
     </row>
-    <row r="8" spans="2:55" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:55" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="100"/>
       <c r="C8" s="100" t="s">
         <v>35</v>
@@ -6144,7 +6144,7 @@
       <c r="BB9"/>
       <c r="BC9"/>
     </row>
-    <row r="10" spans="2:55" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:55" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="104"/>
       <c r="C10" s="67" t="s">
         <v>78</v>
@@ -7582,7 +7582,7 @@
         <v>0.19126558372437868</v>
       </c>
     </row>
-    <row r="18" spans="1:58" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:58" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B18" s="104"/>
       <c r="C18" s="67" t="s">
         <v>78</v>
@@ -7647,7 +7647,7 @@
       <c r="BB18"/>
       <c r="BC18"/>
     </row>
-    <row r="19" spans="1:58" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:58" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B19" s="99"/>
       <c r="C19" s="67" t="s">
         <v>78</v>
@@ -7712,7 +7712,7 @@
       <c r="BB19"/>
       <c r="BC19"/>
     </row>
-    <row r="20" spans="1:58" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:58" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B20" s="99"/>
       <c r="C20" s="67" t="s">
         <v>78</v>
@@ -7778,7 +7778,7 @@
       <c r="BB20"/>
       <c r="BC20"/>
     </row>
-    <row r="21" spans="1:58" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:58" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B21" s="99"/>
       <c r="C21" s="67" t="s">
         <v>78</v>
@@ -7848,7 +7848,7 @@
       <c r="BB21"/>
       <c r="BC21"/>
     </row>
-    <row r="22" spans="1:58" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:58" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B22" s="99"/>
       <c r="C22" s="67" t="s">
         <v>78</v>
@@ -7912,7 +7912,7 @@
       <c r="BB22" s="30"/>
       <c r="BC22"/>
     </row>
-    <row r="23" spans="1:58" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:58" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B23" s="104"/>
       <c r="C23" s="105" t="s">
         <v>78</v>
@@ -7988,7 +7988,7 @@
       </c>
       <c r="S25" s="54"/>
     </row>
-    <row r="26" spans="1:58" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:58" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B26" s="104"/>
       <c r="C26" s="105" t="s">
         <v>78</v>
@@ -8016,7 +8016,7 @@
       <c r="R26" s="121"/>
       <c r="S26" s="54"/>
     </row>
-    <row r="27" spans="1:58" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:58" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B27" s="104"/>
       <c r="C27" s="105" t="s">
         <v>78</v>
@@ -9094,7 +9094,7 @@
         <v>MEUR20</v>
       </c>
     </row>
-    <row r="35" spans="1:55" ht="19.8" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:55" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B35" s="100"/>
       <c r="C35" s="101" t="s">
         <v>78</v>
@@ -9157,7 +9157,7 @@
       <c r="BB35" s="41"/>
       <c r="BC35" s="41"/>
     </row>
-    <row r="36" spans="1:55" ht="19.8" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:55" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B36" s="104"/>
       <c r="C36" s="67" t="s">
         <v>78</v>
@@ -9223,7 +9223,7 @@
       <c r="BB36" s="41"/>
       <c r="BC36" s="41"/>
     </row>
-    <row r="37" spans="1:55" ht="19.8" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:55" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B37" s="104"/>
       <c r="C37" s="67" t="s">
         <v>78</v>
@@ -9290,7 +9290,7 @@
       <c r="BB37"/>
       <c r="BC37"/>
     </row>
-    <row r="38" spans="1:55" ht="19.8" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:55" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B38" s="104"/>
       <c r="C38" s="67" t="s">
         <v>78</v>
@@ -9551,15 +9551,15 @@
       <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.36328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:15" ht="13" x14ac:dyDescent="0.3">
       <c r="B2" s="94" t="s">
         <v>37</v>
       </c>
@@ -9570,7 +9570,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="2:15" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:15" ht="13" x14ac:dyDescent="0.25">
       <c r="B3" s="57" t="s">
         <v>38</v>
       </c>
@@ -9593,7 +9593,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:15" ht="13" x14ac:dyDescent="0.3">
       <c r="B4" s="87" t="s">
         <v>987</v>
       </c>
@@ -9622,7 +9622,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:15" ht="13" x14ac:dyDescent="0.3">
       <c r="B5" s="130" t="s">
         <v>988</v>
       </c>
@@ -9647,7 +9647,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:15" ht="13" x14ac:dyDescent="0.3">
       <c r="B6" s="130" t="s">
         <v>989</v>
       </c>
@@ -9672,7 +9672,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:15" ht="13" x14ac:dyDescent="0.3">
       <c r="B7" s="130" t="s">
         <v>990</v>
       </c>
@@ -9682,7 +9682,7 @@
       <c r="F7" s="133"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:15" ht="13" x14ac:dyDescent="0.3">
       <c r="B8" s="130" t="s">
         <v>991</v>
       </c>
@@ -9692,7 +9692,7 @@
       <c r="F8" s="133"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:15" ht="13" x14ac:dyDescent="0.3">
       <c r="B9" s="130" t="s">
         <v>992</v>
       </c>
@@ -9702,7 +9702,7 @@
       <c r="F9" s="133"/>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:15" ht="13" x14ac:dyDescent="0.3">
       <c r="B10" s="130" t="s">
         <v>937</v>
       </c>
@@ -9712,7 +9712,7 @@
       <c r="F10" s="133"/>
       <c r="G10" s="2"/>
     </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:15" ht="13" x14ac:dyDescent="0.3">
       <c r="B11" s="130" t="s">
         <v>993</v>
       </c>
@@ -9722,7 +9722,7 @@
       <c r="F11" s="133"/>
       <c r="G11" s="2"/>
     </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:15" ht="13" x14ac:dyDescent="0.3">
       <c r="B12" s="130" t="s">
         <v>994</v>
       </c>
@@ -9732,7 +9732,7 @@
       <c r="F12" s="133"/>
       <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:15" ht="13" x14ac:dyDescent="0.3">
       <c r="B13" s="130" t="s">
         <v>995</v>
       </c>
@@ -9742,7 +9742,7 @@
       <c r="F13" s="133"/>
       <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:15" ht="13" x14ac:dyDescent="0.3">
       <c r="B14" s="130" t="s">
         <v>996</v>
       </c>
@@ -9961,19 +9961,19 @@
       <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:26" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>982</v>
       </c>
     </row>
-    <row r="3" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:26" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>983</v>
       </c>
     </row>
-    <row r="5" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:26" ht="13.25" x14ac:dyDescent="0.25">
       <c r="S5" s="41"/>
       <c r="T5" s="41"/>
       <c r="U5" s="41"/>
@@ -9983,7 +9983,7 @@
       <c r="Y5" s="41"/>
       <c r="Z5" s="41"/>
     </row>
-    <row r="6" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:26" ht="13" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>981</v>
       </c>
@@ -9999,7 +9999,7 @@
       <c r="Y6" s="43"/>
       <c r="Z6" s="41"/>
     </row>
-    <row r="7" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:26" ht="13" x14ac:dyDescent="0.3">
       <c r="S7" s="41"/>
       <c r="T7" s="42"/>
       <c r="U7" s="42"/>
@@ -10009,7 +10009,7 @@
       <c r="Y7" s="42"/>
       <c r="Z7" s="42"/>
     </row>
-    <row r="8" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:26" ht="13" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>2010</v>
       </c>
@@ -10034,7 +10034,7 @@
       <c r="Y8" s="125"/>
       <c r="Z8" s="125"/>
     </row>
-    <row r="9" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:26" ht="13" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>2011</v>
       </c>
@@ -10059,7 +10059,7 @@
       <c r="Y9" s="125"/>
       <c r="Z9" s="125"/>
     </row>
-    <row r="10" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:26" ht="13" x14ac:dyDescent="0.3">
       <c r="B10">
         <v>2012</v>
       </c>
@@ -10084,7 +10084,7 @@
       <c r="Y10" s="126"/>
       <c r="Z10" s="126"/>
     </row>
-    <row r="11" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:26" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>2013</v>
       </c>
@@ -10108,7 +10108,7 @@
       <c r="Y11" s="125"/>
       <c r="Z11" s="125"/>
     </row>
-    <row r="12" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:26" ht="13" x14ac:dyDescent="0.3">
       <c r="B12">
         <v>2014</v>
       </c>
@@ -10133,7 +10133,7 @@
       <c r="Y12" s="47"/>
       <c r="Z12" s="47"/>
     </row>
-    <row r="13" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:26" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>2015</v>
       </c>
@@ -10149,7 +10149,7 @@
         <v>1.0675083333333333</v>
       </c>
     </row>
-    <row r="14" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:26" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>2016</v>
       </c>
@@ -10165,7 +10165,7 @@
         <v>1.6065250000000002</v>
       </c>
     </row>
-    <row r="15" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:26" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>2017</v>
       </c>
@@ -10181,7 +10181,7 @@
         <v>1.7234916666666666</v>
       </c>
     </row>
-    <row r="16" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:26" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>2018</v>
       </c>
@@ -10197,7 +10197,7 @@
         <v>1.701225</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>2019</v>
       </c>
@@ -10213,7 +10213,7 @@
         <v>1.7024999999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" ht="13.25" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>2020</v>
       </c>
@@ -15866,9 +15866,9 @@
       <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="15.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:48" x14ac:dyDescent="0.25">
@@ -15876,7 +15876,7 @@
         <v>984</v>
       </c>
     </row>
-    <row r="5" spans="1:48" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:48" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="42" t="s">
         <v>88</v>
       </c>
@@ -15887,7 +15887,7 @@
       <c r="G5" s="43"/>
       <c r="H5" s="43"/>
     </row>
-    <row r="6" spans="1:48" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:48" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="31"/>
       <c r="C6" s="44">
         <v>2010</v>
@@ -15911,7 +15911,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="7" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:48" ht="13" x14ac:dyDescent="0.3">
       <c r="A7" s="45"/>
       <c r="B7" s="46" t="s">
         <v>89</v>
@@ -15945,7 +15945,7 @@
         <v>0.78615548740460983</v>
       </c>
     </row>
-    <row r="8" spans="1:48" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:48" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="45"/>
       <c r="B8" s="48" t="s">
         <v>90</v>
@@ -15979,7 +15979,7 @@
         <v>0.80182435242407102</v>
       </c>
     </row>
-    <row r="9" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:48" ht="13" x14ac:dyDescent="0.3">
       <c r="A9" s="45"/>
       <c r="B9" s="46" t="s">
         <v>91</v>
@@ -16046,7 +16046,7 @@
         <v>0.10769671819564115</v>
       </c>
     </row>
-    <row r="11" spans="1:48" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:48" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="45"/>
       <c r="B11" s="46" t="s">
         <v>93</v>
@@ -16080,7 +16080,7 @@
         <v>0.13431460128400069</v>
       </c>
     </row>
-    <row r="12" spans="1:48" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:48" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="45"/>
       <c r="B12" s="46"/>
       <c r="C12" s="50"/>
@@ -16096,65 +16096,65 @@
       </c>
     </row>
     <row r="14" spans="1:48" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="A15" s="150" t="s">
+    <row r="15" spans="1:48" ht="13" x14ac:dyDescent="0.3">
+      <c r="A15" s="152" t="s">
         <v>95</v>
       </c>
-      <c r="B15" s="150"/>
-      <c r="C15" s="150"/>
-      <c r="D15" s="150"/>
-      <c r="E15" s="150"/>
-      <c r="F15" s="150"/>
-      <c r="H15" s="150" t="s">
+      <c r="B15" s="152"/>
+      <c r="C15" s="152"/>
+      <c r="D15" s="152"/>
+      <c r="E15" s="152"/>
+      <c r="F15" s="152"/>
+      <c r="H15" s="152" t="s">
         <v>96</v>
       </c>
-      <c r="I15" s="150"/>
-      <c r="J15" s="150"/>
-      <c r="K15" s="150"/>
-      <c r="L15" s="150"/>
-      <c r="M15" s="150"/>
-      <c r="O15" s="150" t="s">
+      <c r="I15" s="152"/>
+      <c r="J15" s="152"/>
+      <c r="K15" s="152"/>
+      <c r="L15" s="152"/>
+      <c r="M15" s="152"/>
+      <c r="O15" s="152" t="s">
         <v>97</v>
       </c>
-      <c r="P15" s="150"/>
-      <c r="Q15" s="150"/>
-      <c r="R15" s="150"/>
-      <c r="S15" s="150"/>
-      <c r="T15" s="150"/>
-      <c r="V15" s="150" t="s">
+      <c r="P15" s="152"/>
+      <c r="Q15" s="152"/>
+      <c r="R15" s="152"/>
+      <c r="S15" s="152"/>
+      <c r="T15" s="152"/>
+      <c r="V15" s="152" t="s">
         <v>98</v>
       </c>
-      <c r="W15" s="150"/>
-      <c r="X15" s="150"/>
-      <c r="Y15" s="150"/>
-      <c r="Z15" s="150"/>
-      <c r="AA15" s="150"/>
-      <c r="AC15" s="150" t="s">
+      <c r="W15" s="152"/>
+      <c r="X15" s="152"/>
+      <c r="Y15" s="152"/>
+      <c r="Z15" s="152"/>
+      <c r="AA15" s="152"/>
+      <c r="AC15" s="152" t="s">
         <v>99</v>
       </c>
-      <c r="AD15" s="150"/>
-      <c r="AE15" s="150"/>
-      <c r="AF15" s="150"/>
-      <c r="AG15" s="150"/>
-      <c r="AH15" s="150"/>
-      <c r="AJ15" s="150" t="s">
+      <c r="AD15" s="152"/>
+      <c r="AE15" s="152"/>
+      <c r="AF15" s="152"/>
+      <c r="AG15" s="152"/>
+      <c r="AH15" s="152"/>
+      <c r="AJ15" s="152" t="s">
         <v>100</v>
       </c>
-      <c r="AK15" s="150"/>
-      <c r="AL15" s="150"/>
-      <c r="AM15" s="150"/>
-      <c r="AN15" s="150"/>
-      <c r="AO15" s="150"/>
-      <c r="AQ15" s="149" t="s">
+      <c r="AK15" s="152"/>
+      <c r="AL15" s="152"/>
+      <c r="AM15" s="152"/>
+      <c r="AN15" s="152"/>
+      <c r="AO15" s="152"/>
+      <c r="AQ15" s="151" t="s">
         <v>824</v>
       </c>
-      <c r="AR15" s="149"/>
-      <c r="AS15" s="149"/>
-      <c r="AT15" s="149"/>
-      <c r="AU15" s="149"/>
-      <c r="AV15" s="149"/>
-    </row>
-    <row r="16" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="AR15" s="151"/>
+      <c r="AS15" s="151"/>
+      <c r="AT15" s="151"/>
+      <c r="AU15" s="151"/>
+      <c r="AV15" s="151"/>
+    </row>
+    <row r="16" spans="1:48" ht="13" x14ac:dyDescent="0.3">
       <c r="A16" s="51" t="s">
         <v>101</v>
       </c>
@@ -20102,6 +20102,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100391E4ED4D6B5344984C5B5CBC1A28781" ma:contentTypeVersion="13" ma:contentTypeDescription="Opret et nyt dokument." ma:contentTypeScope="" ma:versionID="a8662b4a95e495bc977359cc4b8d0a5a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6218e30f-ac19-4e1a-9d42-0577826d9887" xmlns:ns3="9bef2f80-48e4-49d2-aa34-66e9d7fcf80f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b72a6a49e693c9bb3f1300811353490c" ns2:_="" ns3:_="">
     <xsd:import namespace="6218e30f-ac19-4e1a-9d42-0577826d9887"/>
@@ -20324,29 +20339,38 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE0421F0-51EF-4FEE-8D79-C499B8BD686A}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5C6FFB9B-9A12-40AA-B62D-7157E8D5CF96}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDEEE354-EE8B-4204-B030-8478E7CEBD45}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDEEE354-EE8B-4204-B030-8478E7CEBD45}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5C6FFB9B-9A12-40AA-B62D-7157E8D5CF96}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE0421F0-51EF-4FEE-8D79-C499B8BD686A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="6218e30f-ac19-4e1a-9d42-0577826d9887"/>
+    <ds:schemaRef ds:uri="9bef2f80-48e4-49d2-aa34-66e9d7fcf80f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>